<commit_message>
Add test for checking garbling in repeat section
</commit_message>
<xml_diff>
--- a/tests/data/test_cases.xlsx
+++ b/tests/data/test_cases.xlsx
@@ -3,19 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326B0DD2-BA56-584D-ACD6-A4C308810B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1C4AE6-8671-0C4D-BA3A-48E2A0E6F6EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29300" yWindow="5120" windowWidth="38840" windowHeight="20040" tabRatio="321" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29300" yWindow="5120" windowWidth="38840" windowHeight="20040" tabRatio="321" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="unsupported_question" sheetId="1" r:id="rId1"/>
     <sheet name="unsupported_function" sheetId="5" r:id="rId2"/>
     <sheet name="infinite_repeat" sheetId="6" r:id="rId3"/>
     <sheet name="nested_repeat" sheetId="7" r:id="rId4"/>
-    <sheet name="choices" sheetId="2" r:id="rId5"/>
-    <sheet name="settings" sheetId="3" r:id="rId6"/>
+    <sheet name="garbling_in_repeat" sheetId="8" r:id="rId5"/>
+    <sheet name="choices" sheetId="2" r:id="rId6"/>
+    <sheet name="settings" sheetId="3" r:id="rId7"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">garbling_in_repeat!$A$1:$N$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">infinite_repeat!$A$1:$N$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">nested_repeat!$A$1:$N$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">unsupported_function!$A$1:$N$4</definedName>
@@ -61,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="131">
   <si>
     <t>type</t>
   </si>
@@ -442,6 +444,18 @@
   </si>
   <si>
     <t>To which continent does this person intend to travel for trip number ${position}?</t>
+  </si>
+  <si>
+    <t>select_one yes.no</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Have you visited it before?</t>
+  </si>
+  <si>
+    <t>ever.visited</t>
   </si>
 </sst>
 </file>
@@ -789,7 +803,70 @@
     <cellStyle name="Normal 4" xfId="45" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
     <cellStyle name="Normal 5" xfId="43" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="27">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1779,6 +1856,270 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I7">
+    <cfRule type="expression" dxfId="26" priority="1">
+      <formula>#REF! ="end repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="2">
+      <formula>#REF!="begin group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="3">
+      <formula>#REF! ="end group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="4">
+      <formula>#REF! = "begin repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="5">
+      <formula>#REF!="begin repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="6">
+      <formula>#REF! ="end repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="7">
+      <formula>#REF!="begin group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="8">
+      <formula>#REF! ="end group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="9">
+      <formula>#REF!="begin repeat"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B43F3330-0DD9-274D-848B-B44033188686}">
+  <dimension ref="A1:Q13"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.6640625" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5" style="13" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="31.83203125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="25.33203125" style="13" customWidth="1"/>
+    <col min="8" max="8" width="19.5" style="15" customWidth="1"/>
+    <col min="9" max="9" width="26.6640625" style="13" customWidth="1"/>
+    <col min="10" max="10" width="22" style="13" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="20.1640625" style="13" customWidth="1"/>
+    <col min="13" max="13" width="18.5" style="13" customWidth="1"/>
+    <col min="14" max="14" width="9.83203125" style="15" customWidth="1"/>
+    <col min="15" max="15" width="18" customWidth="1"/>
+    <col min="16" max="16" width="15.33203125" style="13" customWidth="1"/>
+    <col min="17" max="17" width="21.6640625" style="13" customWidth="1"/>
+    <col min="18" max="16384" width="17.6640625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="8" customFormat="1" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="H2" s="9"/>
+      <c r="N2" s="9"/>
+    </row>
+    <row r="3" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="7"/>
+      <c r="H3" s="9"/>
+      <c r="N3" s="9"/>
+    </row>
+    <row r="4" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="7"/>
+      <c r="H4" s="9"/>
+      <c r="N4" s="9"/>
+    </row>
+    <row r="5" spans="1:17" s="10" customFormat="1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="H5" s="12"/>
+      <c r="N5" s="12"/>
+    </row>
+    <row r="6" spans="1:17" s="10" customFormat="1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="H6" s="12"/>
+      <c r="J6" s="10">
+        <v>5</v>
+      </c>
+      <c r="N6" s="12"/>
+      <c r="O6" s="22"/>
+    </row>
+    <row r="7" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" s="10" customFormat="1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="H8" s="12"/>
+      <c r="J8" s="10">
+        <v>3</v>
+      </c>
+      <c r="N8" s="12"/>
+      <c r="O8" s="22"/>
+    </row>
+    <row r="9" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" s="16" customFormat="1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="17"/>
+      <c r="H11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="21"/>
+    </row>
+    <row r="12" spans="1:17" s="16" customFormat="1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="H12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="21"/>
+    </row>
+    <row r="13" spans="1:17" s="16" customFormat="1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="17"/>
+      <c r="H13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="21"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="I9">
     <cfRule type="expression" dxfId="17" priority="1">
       <formula>#REF! ="end repeat"</formula>
     </cfRule>
@@ -1812,13 +2153,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B43F3330-0DD9-274D-848B-B44033188686}">
-  <dimension ref="A1:Q13"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5F8DC8-A190-2D4B-B31F-1C00AAFC64D8}">
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.6640625" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1950,68 +2291,68 @@
         <v>114</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="D6" s="11"/>
       <c r="H6" s="12"/>
       <c r="J6" s="10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N6" s="12"/>
       <c r="O6" s="22"/>
     </row>
     <row r="7" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="E7" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I8" s="23"/>
+    </row>
+    <row r="9" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="10" customFormat="1" ht="20" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="H8" s="12"/>
-      <c r="J8" s="10">
-        <v>3</v>
-      </c>
-      <c r="N8" s="12"/>
-      <c r="O8" s="22"/>
-    </row>
-    <row r="9" spans="1:17" ht="20" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="I9" s="23" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>120</v>
+        <v>129</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="O10" t="s">
+        <v>30</v>
+      </c>
+      <c r="P10" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="Q10" s="13" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:17" s="16" customFormat="1" ht="20" x14ac:dyDescent="0.25">
@@ -2025,24 +2366,15 @@
     </row>
     <row r="12" spans="1:17" s="16" customFormat="1" ht="20" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>121</v>
+        <v>28</v>
       </c>
       <c r="D12" s="17"/>
       <c r="H12" s="18"/>
       <c r="N12" s="18"/>
       <c r="O12" s="21"/>
     </row>
-    <row r="13" spans="1:17" s="16" customFormat="1" ht="20" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="17"/>
-      <c r="H13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="21"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="I9">
+  <conditionalFormatting sqref="I7:I8">
     <cfRule type="expression" dxfId="8" priority="1">
       <formula>#REF! ="end repeat"</formula>
     </cfRule>
@@ -2076,7 +2408,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D37"/>
@@ -2496,7 +2828,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:E2"/>
@@ -2540,7 +2872,7 @@
       </c>
       <c r="D2" t="str">
         <f ca="1">CONCATENATE(YEAR(TODAY()),TEXT(MONTH(TODAY()),"00"),TEXT(DAY(TODAY()),"00"),TEXT(HOUR(NOW()),"00"),TEXT(MINUTE(NOW()),"00"))</f>
-        <v>202402121107</v>
+        <v>202402121147</v>
       </c>
       <c r="E2" t="s">
         <v>22</v>
@@ -2717,18 +3049,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2750,18 +3082,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{271F0863-BD7A-488E-A3D5-BB6151EB0978}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70EAE8BF-4C5E-4B5F-A4E0-A795DEA1A182}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{271F0863-BD7A-488E-A3D5-BB6151EB0978}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>